<commit_message>
cap nhap danh sach thi admin + layout bai kiem tra + layout ho so
</commit_message>
<xml_diff>
--- a/WebBaiGiang_CKC/UpLoads/Files/CauHoi.xlsx
+++ b/WebBaiGiang_CKC/UpLoads/Files/CauHoi.xlsx
@@ -26,6 +26,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="336">
   <si>
+    <t>ChuongId</t>
+  </si>
+  <si>
     <t>NoiDung</t>
   </si>
   <si>
@@ -1038,9 +1041,6 @@
   </si>
   <si>
     <t>SoLanTraLoiDung</t>
-  </si>
-  <si>
-    <t>ChuongId</t>
   </si>
 </sst>
 </file>
@@ -1363,13 +1363,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="55.28515625" customWidth="1"/>
     <col min="3" max="3" width="64.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" customWidth="1"/>
@@ -1382,34 +1381,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>334</v>
+      </c>
+      <c r="J1" t="s">
         <v>335</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>333</v>
-      </c>
-      <c r="J1" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1417,22 +1416,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -1449,22 +1448,22 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -1481,22 +1480,22 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -1513,22 +1512,22 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -1545,22 +1544,22 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -1577,22 +1576,22 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -1609,22 +1608,22 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -1641,22 +1640,22 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" t="s">
         <v>47</v>
       </c>
-      <c r="C9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" t="s">
-        <v>46</v>
-      </c>
       <c r="G9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -1673,22 +1672,22 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -1705,22 +1704,22 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D11" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H11">
         <v>1</v>
@@ -1737,22 +1736,22 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" t="s">
         <v>69</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>68</v>
       </c>
-      <c r="E12" t="s">
-        <v>67</v>
-      </c>
       <c r="F12" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -1769,22 +1768,22 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C13" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D13" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E13" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F13" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -1801,22 +1800,22 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C14" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D14" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F14" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G14" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H14">
         <v>1</v>
@@ -1833,22 +1832,22 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F15" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G15" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H15">
         <v>1</v>
@@ -1865,22 +1864,22 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C16" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D16" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E16" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F16" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G16" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -1897,22 +1896,22 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" t="s">
         <v>75</v>
       </c>
-      <c r="C17" t="s">
-        <v>63</v>
-      </c>
-      <c r="D17" t="s">
-        <v>72</v>
-      </c>
-      <c r="E17" t="s">
-        <v>74</v>
-      </c>
       <c r="F17" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G17" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H17">
         <v>1</v>
@@ -1929,22 +1928,22 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C18" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D18" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E18" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F18" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G18" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H18">
         <v>1</v>
@@ -1961,22 +1960,22 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" t="s">
+        <v>84</v>
+      </c>
+      <c r="E19" t="s">
+        <v>85</v>
+      </c>
+      <c r="F19" t="s">
         <v>81</v>
       </c>
-      <c r="C19" t="s">
-        <v>82</v>
-      </c>
-      <c r="D19" t="s">
-        <v>83</v>
-      </c>
-      <c r="E19" t="s">
-        <v>84</v>
-      </c>
-      <c r="F19" t="s">
-        <v>80</v>
-      </c>
       <c r="G19" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H19">
         <v>1</v>
@@ -1993,22 +1992,22 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C20" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D20" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E20" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F20" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G20" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -2025,22 +2024,22 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C21" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D21" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E21" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F21" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G21" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H21">
         <v>1</v>
@@ -2057,22 +2056,22 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C22" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D22" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E22" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F22" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G22" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H22">
         <v>1</v>
@@ -2089,22 +2088,22 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D23" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E23" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F23" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G23" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H23">
         <v>1</v>
@@ -2121,22 +2120,22 @@
         <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C24" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D24" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E24" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F24" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G24" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H24">
         <v>1</v>
@@ -2153,22 +2152,22 @@
         <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C25" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D25" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E25" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F25" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G25" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H25">
         <v>1</v>
@@ -2185,22 +2184,22 @@
         <v>2</v>
       </c>
       <c r="B26" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C26" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D26" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E26" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F26" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G26" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H26">
         <v>1</v>
@@ -2217,22 +2216,22 @@
         <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C27" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D27" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E27" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F27" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G27" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H27">
         <v>1</v>
@@ -2249,22 +2248,22 @@
         <v>2</v>
       </c>
       <c r="B28" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D28" t="s">
+        <v>118</v>
+      </c>
+      <c r="E28" t="s">
+        <v>119</v>
+      </c>
+      <c r="F28" t="s">
         <v>120</v>
       </c>
-      <c r="D28" t="s">
-        <v>117</v>
-      </c>
-      <c r="E28" t="s">
-        <v>118</v>
-      </c>
-      <c r="F28" t="s">
-        <v>119</v>
-      </c>
       <c r="G28" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H28">
         <v>1</v>
@@ -2281,22 +2280,22 @@
         <v>2</v>
       </c>
       <c r="B29" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C29" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D29" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E29" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F29" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G29" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H29">
         <v>1</v>
@@ -2313,22 +2312,22 @@
         <v>2</v>
       </c>
       <c r="B30" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C30" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D30" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F30" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G30" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H30">
         <v>1</v>
@@ -2345,22 +2344,22 @@
         <v>2</v>
       </c>
       <c r="B31" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C31" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D31" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E31" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F31" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G31" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H31">
         <v>1</v>
@@ -2377,22 +2376,22 @@
         <v>2</v>
       </c>
       <c r="B32" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C32" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D32" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E32" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F32" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G32" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H32">
         <v>1</v>
@@ -2409,22 +2408,22 @@
         <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C33" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D33" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E33" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F33" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G33" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H33">
         <v>1</v>
@@ -2441,22 +2440,22 @@
         <v>2</v>
       </c>
       <c r="B34" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C34" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D34" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E34" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F34" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G34" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H34">
         <v>1</v>
@@ -2473,22 +2472,22 @@
         <v>2</v>
       </c>
       <c r="B35" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C35" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D35" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E35" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G35" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H35">
         <v>1</v>
@@ -2505,22 +2504,22 @@
         <v>2</v>
       </c>
       <c r="B36" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C36" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D36" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E36" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F36" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G36" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H36">
         <v>1</v>
@@ -2537,22 +2536,22 @@
         <v>2</v>
       </c>
       <c r="B37" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C37" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D37" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E37" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G37" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H37">
         <v>1</v>
@@ -2569,22 +2568,22 @@
         <v>2</v>
       </c>
       <c r="B38" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C38" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D38" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E38" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F38" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G38" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H38">
         <v>1</v>
@@ -2601,22 +2600,22 @@
         <v>2</v>
       </c>
       <c r="B39" t="s">
+        <v>159</v>
+      </c>
+      <c r="C39" t="s">
+        <v>155</v>
+      </c>
+      <c r="D39" t="s">
+        <v>156</v>
+      </c>
+      <c r="E39" t="s">
+        <v>157</v>
+      </c>
+      <c r="F39" t="s">
         <v>158</v>
       </c>
-      <c r="C39" t="s">
-        <v>154</v>
-      </c>
-      <c r="D39" t="s">
-        <v>155</v>
-      </c>
-      <c r="E39" t="s">
-        <v>156</v>
-      </c>
-      <c r="F39" t="s">
-        <v>157</v>
-      </c>
       <c r="G39" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H39">
         <v>1</v>
@@ -2633,22 +2632,22 @@
         <v>2</v>
       </c>
       <c r="B40" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C40" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D40" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E40" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F40" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G40" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H40">
         <v>1</v>
@@ -2665,19 +2664,19 @@
         <v>2</v>
       </c>
       <c r="B41" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C41" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D41" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E41" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="G41" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H41">
         <v>1</v>
@@ -2694,22 +2693,22 @@
         <v>3</v>
       </c>
       <c r="B42" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C42" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D42" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E42" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F42" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="G42" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H42">
         <v>1</v>
@@ -2726,22 +2725,22 @@
         <v>3</v>
       </c>
       <c r="B43" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C43" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D43" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E43" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F43" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G43" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H43">
         <v>1</v>
@@ -2758,22 +2757,22 @@
         <v>3</v>
       </c>
       <c r="B44" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C44" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D44" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E44" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F44" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G44" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H44">
         <v>1</v>
@@ -2790,22 +2789,22 @@
         <v>3</v>
       </c>
       <c r="B45" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C45" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D45" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E45" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F45" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G45" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H45">
         <v>1</v>
@@ -2822,22 +2821,22 @@
         <v>3</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C46" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D46" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E46" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F46" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="G46" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H46">
         <v>1</v>
@@ -2854,22 +2853,22 @@
         <v>3</v>
       </c>
       <c r="B47" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C47" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D47" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E47" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F47" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="G47" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H47">
         <v>1</v>
@@ -2886,22 +2885,22 @@
         <v>3</v>
       </c>
       <c r="B48" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C48" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D48" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E48" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="F48" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="G48" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H48">
         <v>1</v>
@@ -2918,22 +2917,22 @@
         <v>3</v>
       </c>
       <c r="B49" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C49" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E49" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F49" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="G49" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H49">
         <v>1</v>
@@ -2950,22 +2949,22 @@
         <v>3</v>
       </c>
       <c r="B50" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C50" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D50" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E50" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F50" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="G50" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H50">
         <v>1</v>
@@ -2982,22 +2981,22 @@
         <v>3</v>
       </c>
       <c r="B51" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C51" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D51" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E51" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F51" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G51" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H51">
         <v>1</v>
@@ -3014,22 +3013,22 @@
         <v>3</v>
       </c>
       <c r="B52" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C52" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D52" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E52" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="F52" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="G52" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H52">
         <v>1</v>
@@ -3046,22 +3045,22 @@
         <v>3</v>
       </c>
       <c r="B53" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C53" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D53" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="E53" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="F53" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="G53" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H53">
         <v>1</v>
@@ -3078,22 +3077,22 @@
         <v>3</v>
       </c>
       <c r="B54" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C54" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D54" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="E54" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F54" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G54" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H54">
         <v>1</v>
@@ -3110,22 +3109,22 @@
         <v>3</v>
       </c>
       <c r="B55" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C55" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D55" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E55" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="F55" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="G55" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H55">
         <v>1</v>
@@ -3142,22 +3141,22 @@
         <v>3</v>
       </c>
       <c r="B56" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C56" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D56" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E56" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F56" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="G56" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H56">
         <v>1</v>
@@ -3174,22 +3173,22 @@
         <v>3</v>
       </c>
       <c r="B57" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C57" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D57" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="E57" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="F57" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="G57" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H57">
         <v>1</v>
@@ -3206,22 +3205,22 @@
         <v>3</v>
       </c>
       <c r="B58" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C58" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D58" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E58" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="F58" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="G58" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H58">
         <v>1</v>
@@ -3238,22 +3237,22 @@
         <v>3</v>
       </c>
       <c r="B59" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C59" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D59" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="E59" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="F59" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="G59" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H59">
         <v>1</v>
@@ -3270,22 +3269,22 @@
         <v>3</v>
       </c>
       <c r="B60" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C60" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D60" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E60" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="F60" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="G60" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H60">
         <v>1</v>
@@ -3302,22 +3301,22 @@
         <v>3</v>
       </c>
       <c r="B61" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C61" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D61" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="E61" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="F61" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="G61" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H61">
         <v>1</v>
@@ -3334,22 +3333,22 @@
         <v>4</v>
       </c>
       <c r="B62" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C62" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D62" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="E62" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="F62" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="G62" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H62">
         <v>1</v>
@@ -3366,22 +3365,22 @@
         <v>4</v>
       </c>
       <c r="B63" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C63" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D63" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="E63" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="F63" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="G63" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H63">
         <v>1</v>
@@ -3398,22 +3397,22 @@
         <v>4</v>
       </c>
       <c r="B64" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C64" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D64" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="E64" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="F64" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G64" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H64">
         <v>1</v>
@@ -3430,22 +3429,22 @@
         <v>4</v>
       </c>
       <c r="B65" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C65" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D65" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E65" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="F65" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G65" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H65">
         <v>1</v>
@@ -3462,22 +3461,22 @@
         <v>4</v>
       </c>
       <c r="B66" t="s">
+        <v>273</v>
+      </c>
+      <c r="C66" t="s">
+        <v>274</v>
+      </c>
+      <c r="D66" t="s">
+        <v>275</v>
+      </c>
+      <c r="E66" t="s">
+        <v>276</v>
+      </c>
+      <c r="F66" t="s">
         <v>272</v>
       </c>
-      <c r="C66" t="s">
-        <v>273</v>
-      </c>
-      <c r="D66" t="s">
-        <v>274</v>
-      </c>
-      <c r="E66" t="s">
-        <v>275</v>
-      </c>
-      <c r="F66" t="s">
-        <v>271</v>
-      </c>
       <c r="G66" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H66">
         <v>1</v>
@@ -3494,22 +3493,22 @@
         <v>4</v>
       </c>
       <c r="B67" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C67" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D67" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="E67" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="F67" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="G67" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H67">
         <v>1</v>
@@ -3526,22 +3525,22 @@
         <v>4</v>
       </c>
       <c r="B68" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C68" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D68" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E68" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="F68" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="G68" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H68">
         <v>1</v>
@@ -3558,22 +3557,22 @@
         <v>4</v>
       </c>
       <c r="B69" t="s">
+        <v>287</v>
+      </c>
+      <c r="C69" t="s">
+        <v>283</v>
+      </c>
+      <c r="D69" t="s">
+        <v>284</v>
+      </c>
+      <c r="E69" t="s">
+        <v>285</v>
+      </c>
+      <c r="F69" t="s">
         <v>286</v>
       </c>
-      <c r="C69" t="s">
-        <v>282</v>
-      </c>
-      <c r="D69" t="s">
-        <v>283</v>
-      </c>
-      <c r="E69" t="s">
-        <v>284</v>
-      </c>
-      <c r="F69" t="s">
-        <v>285</v>
-      </c>
       <c r="G69" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H69">
         <v>1</v>
@@ -3590,22 +3589,22 @@
         <v>4</v>
       </c>
       <c r="B70" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C70" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D70" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="E70" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="F70" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="G70" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H70">
         <v>1</v>
@@ -3622,22 +3621,22 @@
         <v>4</v>
       </c>
       <c r="B71" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C71" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D71" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E71" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="F71" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="G71" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H71">
         <v>1</v>
@@ -3654,22 +3653,22 @@
         <v>4</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C72" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D72" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="E72" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="F72" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="G72" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H72">
         <v>1</v>
@@ -3686,22 +3685,22 @@
         <v>4</v>
       </c>
       <c r="B73" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C73" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D73" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="E73" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="F73" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="G73" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H73">
         <v>1</v>
@@ -3718,22 +3717,22 @@
         <v>4</v>
       </c>
       <c r="B74" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C74" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D74" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="E74" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="F74" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="G74" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H74">
         <v>1</v>
@@ -3750,22 +3749,22 @@
         <v>4</v>
       </c>
       <c r="B75" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C75" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D75" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="F75" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="G75" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H75">
         <v>1</v>
@@ -3782,22 +3781,22 @@
         <v>4</v>
       </c>
       <c r="B76" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C76" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D76" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E76" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="F76" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="G76" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H76">
         <v>1</v>
@@ -3814,22 +3813,22 @@
         <v>4</v>
       </c>
       <c r="B77" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C77" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D77" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E77" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="F77" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="G77" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H77">
         <v>1</v>
@@ -3846,22 +3845,22 @@
         <v>4</v>
       </c>
       <c r="B78" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C78" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D78" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E78" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="F78" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="G78" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H78">
         <v>1</v>
@@ -3878,22 +3877,22 @@
         <v>4</v>
       </c>
       <c r="B79" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C79" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D79" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="E79" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="F79" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="G79" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H79">
         <v>1</v>
@@ -3910,22 +3909,22 @@
         <v>4</v>
       </c>
       <c r="B80" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C80" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D80" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="E80" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="F80" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="G80" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H80">
         <v>1</v>
@@ -3942,22 +3941,22 @@
         <v>4</v>
       </c>
       <c r="B81" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C81" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D81" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="E81" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="F81" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="G81" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H81">
         <v>1</v>

</xml_diff>